<commit_message>
Pridani zjisteni minima ceny
</commit_message>
<xml_diff>
--- a/produkty.xlsx
+++ b/produkty.xlsx
@@ -8,6 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="18 - inSPORTline Odino" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="19 - Produkt" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="20 - Marshall Major IV Bluetoo" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="21 - PlayStation 5 Slim" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="22 - Marshall Major IV Bluetoo" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -136,7 +140,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="1"/>
+  <style val="13"/>
   <chart>
     <title>
       <tx>
@@ -174,12 +178,468 @@
           </marker>
           <cat>
             <numRef>
-              <f>'18 - inSPORTline Odino'!$A$4:$A$36</f>
+              <f>'18 - inSPORTline Odino'!$A$4:$A$109</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'18 - inSPORTline Odino'!$B$4:$B$36</f>
+              <f>'18 - inSPORTline Odino'!$B$4:$B$109</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Datum</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Cena</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Historie cen</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'19 - Produkt'!$A$4:$A$109</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'19 - Produkt'!$B$4:$B$109</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Datum</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Cena</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Historie cen</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'20 - Marshall Major IV Bluetoo'!$A$4:$A$109</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'20 - Marshall Major IV Bluetoo'!$B$4:$B$109</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Datum</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Cena</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Historie cen</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'21 - PlayStation 5 Slim'!$A$4:$A$109</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'21 - PlayStation 5 Slim'!$B$4:$B$109</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Datum</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Cena</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Historie cen</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'22 - Marshall Major IV Bluetoo'!$A$4:$A$109</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'22 - Marshall Major IV Bluetoo'!$B$4:$B$109</f>
             </numRef>
           </val>
         </ser>
@@ -249,6 +709,114 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -564,7 +1132,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -574,7 +1142,7 @@
   <cols>
     <col width="21" customWidth="1" min="1" max="1"/>
     <col width="128" customWidth="1" min="2" max="2"/>
-    <col width="6" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -588,6 +1156,11 @@
           <t>inSPORTline Odino</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Moje cena</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -599,6 +1172,9 @@
         <is>
           <t>https://chytre-hodinky.heureka.cz/insportline-odino/?utm_source=heureka&amp;utm_medium=productad#prehled/?sort-filter=lowest_price</t>
         </is>
+      </c>
+      <c r="C2" t="n">
+        <v>5500</v>
       </c>
     </row>
     <row r="3"/>
@@ -611,9 +1187,6 @@
       <c r="B4" s="2" t="n">
         <v>1779</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>5500</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -624,9 +1197,6 @@
       <c r="B5" t="n">
         <v>1779</v>
       </c>
-      <c r="C5" t="n">
-        <v>5500</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -637,9 +1207,6 @@
       <c r="B6" t="n">
         <v>1779</v>
       </c>
-      <c r="C6" t="n">
-        <v>5500</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -650,9 +1217,6 @@
       <c r="B7" t="n">
         <v>1779</v>
       </c>
-      <c r="C7" t="n">
-        <v>5500</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -663,9 +1227,6 @@
       <c r="B8" t="n">
         <v>1779</v>
       </c>
-      <c r="C8" t="n">
-        <v>5500</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -676,9 +1237,6 @@
       <c r="B9" t="n">
         <v>1779</v>
       </c>
-      <c r="C9" t="n">
-        <v>5500</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -689,9 +1247,6 @@
       <c r="B10" t="n">
         <v>1779</v>
       </c>
-      <c r="C10" t="n">
-        <v>5500</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -702,9 +1257,6 @@
       <c r="B11" t="n">
         <v>1779</v>
       </c>
-      <c r="C11" t="n">
-        <v>5500</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -715,9 +1267,6 @@
       <c r="B12" t="n">
         <v>1779</v>
       </c>
-      <c r="C12" t="n">
-        <v>5500</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -728,9 +1277,6 @@
       <c r="B13" t="n">
         <v>1779</v>
       </c>
-      <c r="C13" t="n">
-        <v>5500</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -741,9 +1287,6 @@
       <c r="B14" t="n">
         <v>1779</v>
       </c>
-      <c r="C14" t="n">
-        <v>5500</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -754,9 +1297,6 @@
       <c r="B15" t="n">
         <v>1779</v>
       </c>
-      <c r="C15" t="n">
-        <v>5500</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -767,9 +1307,6 @@
       <c r="B16" t="n">
         <v>1779</v>
       </c>
-      <c r="C16" t="n">
-        <v>5500</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -780,9 +1317,6 @@
       <c r="B17" t="n">
         <v>1779</v>
       </c>
-      <c r="C17" t="n">
-        <v>5500</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -793,8 +1327,1108 @@
       <c r="B18" t="n">
         <v>1779</v>
       </c>
-      <c r="C18" t="n">
-        <v>5500</v>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-12-26T20:54:13</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-12-26T20:56:14</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-12-27T13:27:26</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-12-27T13:47:25</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-12-27T13:49:25</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-12-27T17:27:04</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-12-28T18:28:57</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-12-31T18:08:59</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2026-01-01T21:00:47</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2026-01-03T21:48:44</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2026-01-06T20:22:02</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2026-01-07T20:38:27</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2026-01-10T19:49:20</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:07:48</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:08:53</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:10:38</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2026-01-11T19:34:49</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2026-01-16T18:37:15</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="79" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Produkt:</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Moje cena</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Heureka URL:</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://feny.heureka.cz/rowenta-cv5831f0_3/#prehled/?sort-filter=lowest_price</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>2025-12-24T22:14:25</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-12-25T16:55:53</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-12-25T16:58:50</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-12-25T17:00:28</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-12-25T17:01:57</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-12-25T17:30:43</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-12-25T17:31:39</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-12-26T11:28:41</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-12-26T11:59:39</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-12-26T12:01:16</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-12-26T20:54:33</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-12-26T20:56:27</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-12-27T13:27:49</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-12-27T13:47:49</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-12-27T13:49:48</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-12-27T17:27:18</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-12-28T18:29:11</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-12-31T18:09:11</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2026-01-01T21:01:01</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2026-01-03T21:48:58</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2026-01-06T20:22:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2026-01-07T20:39:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2026-01-10T19:49:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:08:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:09:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:11:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2026-01-11T19:35:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2026-01-16T18:37:48</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="93" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Produkt:</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Marshall Major IV Bluetooth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Moje cena</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Heureka URL:</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://sluchatka.heureka.cz/marshall-major-iv-bluetooth/#prehled/?sort-filter=lowest_price</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>2025-12-25T17:00:42</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-12-25T17:02:10</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-12-25T17:30:56</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-12-25T17:31:51</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-12-26T11:29:04</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-12-26T12:00:05</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-12-26T12:01:39</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-12-26T20:54:50</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-12-26T20:56:42</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-12-27T13:28:13</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-12-27T13:48:16</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-12-27T13:50:11</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-12-27T17:27:32</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-12-28T18:29:25</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-12-31T18:09:24</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2026-01-01T21:01:16</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2026-01-03T21:49:14</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2026-01-07T20:39:44</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2026-01-10T19:50:23</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:09:57</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:11:42</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2026-01-11T19:36:01</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2026-01-16T18:38:20</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="63" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Produkt:</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PlayStation 5 Slim</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Moje cena</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Heureka URL:</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://herni-konzole.heureka.cz/playstation-5-slim/#prehled/</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>2025-12-27T13:48:42</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>11221</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-12-27T13:50:37</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>11221</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-12-27T17:27:47</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>11221</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-12-28T18:29:42</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>13989</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-12-31T18:09:42</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>12390</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2026-01-01T21:01:30</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>12390</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2026-01-03T21:49:30</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>11990</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2026-01-07T20:40:07</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>12328</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2026-01-10T19:50:39</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>12449</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:11:58</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>12449</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2026-01-11T19:36:27</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>12449</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2026-01-16T18:38:44</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>12423</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="68" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Produkt:</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Marshall Major IV Bluetooth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Moje cena</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Heureka URL:</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://sluchatka.heureka.cz/marshall-major-iv-bluetooth/#prehled/</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>2025-12-28T18:29:57</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-12-31T18:09:54</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-01-01T21:01:46</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2026-01-03T21:49:46</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2026-01-07T20:40:31</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2026-01-10T19:50:58</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:12:17</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2026-01-11T19:36:44</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2026-01-16T18:39:07</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dodělání act_price + zapsaní všech statistik do excelu
</commit_message>
<xml_diff>
--- a/produkty.xlsx
+++ b/produkty.xlsx
@@ -178,12 +178,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'18 - inSPORTline Odino'!$A$4:$A$109</f>
+              <f>'18 - inSPORTline Odino'!$A$4:$A$124</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'18 - inSPORTline Odino'!$B$4:$B$109</f>
+              <f>'18 - inSPORTline Odino'!$B$4:$B$124</f>
             </numRef>
           </val>
         </ser>
@@ -292,12 +292,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'19 - Produkt'!$A$4:$A$109</f>
+              <f>'19 - Produkt'!$A$4:$A$124</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'19 - Produkt'!$B$4:$B$109</f>
+              <f>'19 - Produkt'!$B$4:$B$124</f>
             </numRef>
           </val>
         </ser>
@@ -406,12 +406,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'20 - Marshall Major IV Bluetoo'!$A$4:$A$109</f>
+              <f>'20 - Marshall Major IV Bluetoo'!$A$4:$A$124</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'20 - Marshall Major IV Bluetoo'!$B$4:$B$109</f>
+              <f>'20 - Marshall Major IV Bluetoo'!$B$4:$B$124</f>
             </numRef>
           </val>
         </ser>
@@ -520,12 +520,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'21 - PlayStation 5 Slim'!$A$4:$A$109</f>
+              <f>'21 - PlayStation 5 Slim'!$A$4:$A$124</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'21 - PlayStation 5 Slim'!$B$4:$B$109</f>
+              <f>'21 - PlayStation 5 Slim'!$B$4:$B$124</f>
             </numRef>
           </val>
         </ser>
@@ -634,12 +634,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'22 - Marshall Major IV Bluetoo'!$A$4:$A$109</f>
+              <f>'22 - Marshall Major IV Bluetoo'!$A$4:$A$124</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'22 - Marshall Major IV Bluetoo'!$B$4:$B$109</f>
+              <f>'22 - Marshall Major IV Bluetoo'!$B$4:$B$124</f>
             </numRef>
           </val>
         </ser>
@@ -1132,7 +1132,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1143,6 +1143,8 @@
     <col width="21" customWidth="1" min="1" max="1"/>
     <col width="128" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1161,6 +1163,11 @@
           <t>Moje cena</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Statistiky</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1176,62 +1183,63 @@
       <c r="C2" t="n">
         <v>5500</v>
       </c>
-    </row>
-    <row r="3"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Min cena</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Max cena</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1849</v>
+      </c>
+    </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>2025-12-23T21:16:46</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>1779</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Průměrná cena</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1800.212121212121</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2025-12-23T21:23:16</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1779</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2025-12-23T21:24:22</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1779</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2025-12-23T21:26:19</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>1779</v>
-      </c>
-    </row>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Aktuální cena</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7"/>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2025-12-23T21:33:45</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1779</v>
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Datum</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-24T22:14:11</t>
+          <t>2025-12-23T21:16:46</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1241,7 +1249,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-25T16:55:41</t>
+          <t>2025-12-23T21:23:16</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1251,7 +1259,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-25T16:58:38</t>
+          <t>2025-12-23T21:24:22</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1261,7 +1269,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-25T17:00:16</t>
+          <t>2025-12-23T21:26:19</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1271,7 +1279,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-25T17:01:45</t>
+          <t>2025-12-23T21:33:45</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1281,7 +1289,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-25T17:30:30</t>
+          <t>2025-12-24T22:14:11</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1291,7 +1299,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-25T17:31:27</t>
+          <t>2025-12-25T16:55:41</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1301,7 +1309,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-26T11:28:17</t>
+          <t>2025-12-25T16:58:38</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1311,7 +1319,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-26T11:59:17</t>
+          <t>2025-12-25T17:00:16</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1321,7 +1329,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-26T12:00:48</t>
+          <t>2025-12-25T17:01:45</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1331,7 +1339,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-26T20:54:13</t>
+          <t>2025-12-25T17:30:30</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1341,7 +1349,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-26T20:56:14</t>
+          <t>2025-12-25T17:31:27</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1351,7 +1359,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-27T13:27:26</t>
+          <t>2025-12-26T11:28:17</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1361,7 +1369,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-27T13:47:25</t>
+          <t>2025-12-26T11:59:17</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1371,7 +1379,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-27T13:49:25</t>
+          <t>2025-12-26T12:00:48</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1381,7 +1389,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-27T17:27:04</t>
+          <t>2025-12-26T20:54:13</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1391,7 +1399,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-28T18:28:57</t>
+          <t>2025-12-26T20:56:14</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1401,7 +1409,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-31T18:08:59</t>
+          <t>2025-12-27T13:27:26</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1411,57 +1419,57 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-01T21:00:47</t>
+          <t>2025-12-27T13:47:25</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1849</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-03T21:48:44</t>
+          <t>2025-12-27T13:49:25</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1849</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-06T20:22:02</t>
+          <t>2025-12-27T17:27:04</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1849</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-07T20:38:27</t>
+          <t>2025-12-28T18:28:57</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1849</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-10T19:49:20</t>
+          <t>2025-12-31T18:08:59</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1849</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-10T20:07:48</t>
+          <t>2026-01-01T21:00:47</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1471,7 +1479,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-10T20:08:53</t>
+          <t>2026-01-03T21:48:44</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1481,7 +1489,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-10T20:10:38</t>
+          <t>2026-01-06T20:22:02</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1491,7 +1499,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-11T19:34:49</t>
+          <t>2026-01-07T20:38:27</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1501,10 +1509,90 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>2026-01-10T19:49:20</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:07:48</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:08:53</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:10:38</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2026-01-11T19:34:49</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
           <t>2026-01-16T18:37:15</t>
         </is>
       </c>
-      <c r="B36" t="n">
+      <c r="B41" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2026-01-17T09:58:00</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2026-01-17T10:03:11</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2026-01-17T10:18:15</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
         <v>1849</v>
       </c>
     </row>
@@ -1520,7 +1608,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1531,6 +1619,8 @@
     <col width="21" customWidth="1" min="1" max="1"/>
     <col width="79" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="7" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1544,6 +1634,11 @@
           <t>Moje cena</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Statistiky</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1559,62 +1654,60 @@
       <c r="C2" t="n">
         <v>500</v>
       </c>
-    </row>
-    <row r="3"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Min cena</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Max cena</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>778</v>
+      </c>
+    </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>2025-12-24T22:14:25</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Průměrná cena</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>778</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2025-12-25T16:55:53</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2025-12-25T16:58:50</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2025-12-25T17:00:28</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>778</v>
-      </c>
-    </row>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Aktuální cena</t>
+        </is>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7"/>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2025-12-25T17:01:57</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>778</v>
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Datum</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-25T17:30:43</t>
+          <t>2025-12-24T22:14:25</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1624,7 +1717,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-25T17:31:39</t>
+          <t>2025-12-25T16:55:53</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1634,7 +1727,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-26T11:28:41</t>
+          <t>2025-12-25T16:58:50</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1644,7 +1737,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-26T11:59:39</t>
+          <t>2025-12-25T17:00:28</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1654,7 +1747,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-26T12:01:16</t>
+          <t>2025-12-25T17:01:57</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1664,7 +1757,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-26T20:54:33</t>
+          <t>2025-12-25T17:30:43</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1674,7 +1767,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-26T20:56:27</t>
+          <t>2025-12-25T17:31:39</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1684,7 +1777,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-27T13:27:49</t>
+          <t>2025-12-26T11:28:41</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1694,7 +1787,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-27T13:47:49</t>
+          <t>2025-12-26T11:59:39</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1704,7 +1797,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-27T13:49:48</t>
+          <t>2025-12-26T12:01:16</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1714,7 +1807,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-27T17:27:18</t>
+          <t>2025-12-26T20:54:33</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1724,7 +1817,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-28T18:29:11</t>
+          <t>2025-12-26T20:56:27</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1734,7 +1827,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-31T18:09:11</t>
+          <t>2025-12-27T13:27:49</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1744,7 +1837,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-01T21:01:01</t>
+          <t>2025-12-27T13:47:49</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1754,7 +1847,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-03T21:48:58</t>
+          <t>2025-12-27T13:49:48</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1764,56 +1857,127 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-06T20:22:38</t>
-        </is>
+          <t>2025-12-27T17:27:18</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>778</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-07T20:39:05</t>
-        </is>
+          <t>2025-12-28T18:29:11</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>778</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-10T19:49:51</t>
-        </is>
+          <t>2025-12-31T18:09:11</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>778</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-10T20:08:21</t>
-        </is>
+          <t>2026-01-01T21:01:01</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>778</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-10T20:09:24</t>
-        </is>
+          <t>2026-01-03T21:48:58</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>778</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-10T20:11:07</t>
+          <t>2026-01-06T20:22:38</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-11T19:35:22</t>
+          <t>2026-01-07T20:39:05</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>2026-01-10T19:49:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:08:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:09:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:11:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2026-01-11T19:35:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
           <t>2026-01-16T18:37:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2026-01-17T09:58:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2026-01-17T10:03:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2026-01-17T10:18:48</t>
         </is>
       </c>
     </row>
@@ -1829,7 +1993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1840,6 +2004,8 @@
     <col width="21" customWidth="1" min="1" max="1"/>
     <col width="93" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1858,6 +2024,11 @@
           <t>Moje cena</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Statistiky</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1873,102 +2044,103 @@
       <c r="C2" t="n">
         <v>1200</v>
       </c>
-    </row>
-    <row r="3"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Min cena</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Max cena</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1399</v>
+      </c>
+    </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>2025-12-25T17:00:42</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>1399</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Průměrná cena</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1391.95652173913</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2025-12-25T17:02:10</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1399</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2025-12-25T17:30:56</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1399</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2025-12-25T17:31:51</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>1399</v>
-      </c>
-    </row>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Aktuální cena</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7"/>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2025-12-26T11:29:04</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1390</v>
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Datum</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-26T12:00:05</t>
+          <t>2025-12-25T17:00:42</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1390</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-26T12:01:39</t>
+          <t>2025-12-25T17:02:10</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1390</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-26T20:54:50</t>
+          <t>2025-12-25T17:30:56</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1390</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-26T20:56:42</t>
+          <t>2025-12-25T17:31:51</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1390</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-27T13:28:13</t>
+          <t>2025-12-26T11:29:04</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1978,7 +2150,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-27T13:48:16</t>
+          <t>2025-12-26T12:00:05</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1988,7 +2160,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-27T13:50:11</t>
+          <t>2025-12-26T12:01:39</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1998,7 +2170,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-27T17:27:32</t>
+          <t>2025-12-26T20:54:50</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -2008,7 +2180,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-28T18:29:25</t>
+          <t>2025-12-26T20:56:42</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -2018,17 +2190,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-31T18:09:24</t>
+          <t>2025-12-27T13:28:13</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1399</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-01T21:01:16</t>
+          <t>2025-12-27T13:48:16</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -2038,7 +2210,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-03T21:49:14</t>
+          <t>2025-12-27T13:50:11</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -2048,7 +2220,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-07T20:39:44</t>
+          <t>2025-12-27T17:27:32</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -2058,7 +2230,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-10T19:50:23</t>
+          <t>2025-12-28T18:29:25</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -2068,17 +2240,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-10T20:09:57</t>
+          <t>2025-12-31T18:09:24</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1390</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-10T20:11:42</t>
+          <t>2026-01-01T21:01:16</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -2088,7 +2260,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-11T19:36:01</t>
+          <t>2026-01-03T21:49:14</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -2098,11 +2270,91 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-16T18:38:20</t>
+          <t>2026-01-07T20:39:44</t>
         </is>
       </c>
       <c r="B26" t="n">
         <v>1390</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2026-01-10T19:50:23</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:09:57</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:11:42</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2026-01-11T19:36:01</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2026-01-16T18:38:20</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2026-01-17T09:59:08</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2026-01-17T10:04:19</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2026-01-17T10:19:20</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1399</v>
       </c>
     </row>
   </sheetData>
@@ -2117,7 +2369,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2128,6 +2380,8 @@
     <col width="21" customWidth="1" min="1" max="1"/>
     <col width="63" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="9" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2146,6 +2400,11 @@
           <t>Moje cena</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Statistiky</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -2161,125 +2420,206 @@
       <c r="C2" t="n">
         <v>500</v>
       </c>
-    </row>
-    <row r="3"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Min cena</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>11221</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Max cena</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>13989</v>
+      </c>
+    </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>2025-12-27T13:48:42</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>11221</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Průměrná cena</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>12210</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2025-12-27T13:50:37</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>11221</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2025-12-27T17:27:47</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>11221</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2025-12-28T18:29:42</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>13989</v>
-      </c>
-    </row>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Aktuální cena</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>12423</v>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7"/>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2025-12-31T18:09:42</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>12390</v>
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Datum</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-01T21:01:30</t>
+          <t>2025-12-27T13:48:42</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>12390</v>
+        <v>11221</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-03T21:49:30</t>
+          <t>2025-12-27T13:50:37</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>11990</v>
+        <v>11221</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-07T20:40:07</t>
+          <t>2025-12-27T17:27:47</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>12328</v>
+        <v>11221</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-10T19:50:39</t>
+          <t>2025-12-28T18:29:42</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>12449</v>
+        <v>13989</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-10T20:11:58</t>
+          <t>2025-12-31T18:09:42</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>12449</v>
+        <v>12390</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-11T19:36:27</t>
+          <t>2026-01-01T21:01:30</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>12449</v>
+        <v>12390</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>2026-01-03T21:49:30</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>11990</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2026-01-07T20:40:07</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>12328</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2026-01-10T19:50:39</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>12449</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:11:58</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>12449</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2026-01-11T19:36:27</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>12449</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>2026-01-16T18:38:44</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="B20" t="n">
+        <v>12423</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2026-01-17T09:59:31</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>12423</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2026-01-17T10:04:38</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>12423</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2026-01-17T10:19:39</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
         <v>12423</v>
       </c>
     </row>
@@ -2295,7 +2635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2306,6 +2646,8 @@
     <col width="21" customWidth="1" min="1" max="1"/>
     <col width="68" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="19" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2324,6 +2666,11 @@
           <t>Moje cena</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Statistiky</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -2339,62 +2686,63 @@
       <c r="C2" t="n">
         <v>55</v>
       </c>
-    </row>
-    <row r="3"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Min cena</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Max cena</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1479</v>
+      </c>
+    </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>2025-12-28T18:29:57</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>1479</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Průměrná cena</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1469.111111111111</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2025-12-31T18:09:54</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1479</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2026-01-01T21:01:46</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1479</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2026-01-03T21:49:46</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>1479</v>
-      </c>
-    </row>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Aktuální cena</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7"/>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2026-01-07T20:40:31</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1479</v>
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Datum</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-10T19:50:58</t>
+          <t>2025-12-28T18:29:57</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -2404,7 +2752,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-10T20:12:17</t>
+          <t>2025-12-31T18:09:54</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -2414,7 +2762,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-11T19:36:44</t>
+          <t>2026-01-01T21:01:46</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -2424,11 +2772,91 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>2026-01-03T21:49:46</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2026-01-07T20:40:31</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2026-01-10T19:50:58</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2026-01-10T20:12:17</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2026-01-11T19:36:44</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>2026-01-16T18:39:07</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="B17" t="n">
         <v>1390</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2026-01-17T09:59:53</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2026-01-17T10:04:58</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2026-01-17T10:19:57</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gitignore a dodelani odesilani mailu
</commit_message>
<xml_diff>
--- a/produkty.xlsx
+++ b/produkty.xlsx
@@ -178,12 +178,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'18 - inSPORTline Odino'!$A$4:$A$124</f>
+              <f>'18 - inSPORTline Odino'!$A$4:$A$149</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'18 - inSPORTline Odino'!$B$4:$B$124</f>
+              <f>'18 - inSPORTline Odino'!$B$4:$B$149</f>
             </numRef>
           </val>
         </ser>
@@ -292,12 +292,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'19 - Produkt'!$A$4:$A$124</f>
+              <f>'19 - Produkt'!$A$4:$A$149</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'19 - Produkt'!$B$4:$B$124</f>
+              <f>'19 - Produkt'!$B$4:$B$149</f>
             </numRef>
           </val>
         </ser>
@@ -406,12 +406,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'20 - Marshall Major IV Bluetoo'!$A$4:$A$124</f>
+              <f>'20 - Marshall Major IV Bluetoo'!$A$4:$A$149</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'20 - Marshall Major IV Bluetoo'!$B$4:$B$124</f>
+              <f>'20 - Marshall Major IV Bluetoo'!$B$4:$B$149</f>
             </numRef>
           </val>
         </ser>
@@ -520,12 +520,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'21 - PlayStation 5 Slim'!$A$4:$A$124</f>
+              <f>'21 - PlayStation 5 Slim'!$A$4:$A$149</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'21 - PlayStation 5 Slim'!$B$4:$B$124</f>
+              <f>'21 - PlayStation 5 Slim'!$B$4:$B$149</f>
             </numRef>
           </val>
         </ser>
@@ -634,12 +634,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'22 - Marshall Major IV Bluetoo'!$A$4:$A$124</f>
+              <f>'22 - Marshall Major IV Bluetoo'!$A$4:$A$149</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'22 - Marshall Major IV Bluetoo'!$B$4:$B$124</f>
+              <f>'22 - Marshall Major IV Bluetoo'!$B$4:$B$149</f>
             </numRef>
           </val>
         </ser>
@@ -1132,7 +1132,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1144,7 +1144,7 @@
     <col width="128" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="9" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1800.212121212121</v>
+        <v>1808.75</v>
       </c>
     </row>
     <row r="5">
@@ -1593,6 +1593,56 @@
         </is>
       </c>
       <c r="B44" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:43:18</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:48:43</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:54:10</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:55:50</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:58:52</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
         <v>1849</v>
       </c>
     </row>
@@ -1608,7 +1658,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1981,6 +2031,41 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:43:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:49:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:54:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:56:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:59:16</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
@@ -1993,7 +2078,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2005,7 +2090,7 @@
     <col width="93" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2070,7 +2155,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1391.95652173913</v>
+        <v>1393.6</v>
       </c>
     </row>
     <row r="5">
@@ -2080,7 +2165,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1390</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="6"/>
@@ -2354,6 +2439,56 @@
         </is>
       </c>
       <c r="B34" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:44:07</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:49:31</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:54:57</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:56:37</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:59:43</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
         <v>1399</v>
       </c>
     </row>
@@ -2369,7 +2504,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2381,7 +2516,7 @@
     <col width="63" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="9" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2446,7 +2581,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>12210</v>
+        <v>12288.47368421053</v>
       </c>
     </row>
     <row r="5">
@@ -2620,6 +2755,56 @@
         </is>
       </c>
       <c r="B23" t="n">
+        <v>12423</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:44:16</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>12423</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:49:49</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>12423</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:55:10</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>12423</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:56:46</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>12423</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:59:52</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
         <v>12423</v>
       </c>
     </row>
@@ -2635,7 +2820,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2647,7 +2832,7 @@
     <col width="68" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="19" customWidth="1" min="5" max="5"/>
+    <col width="11" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2712,7 +2897,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1469.111111111111</v>
+        <v>1438.4375</v>
       </c>
     </row>
     <row r="5">
@@ -2722,7 +2907,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1390</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="6"/>
@@ -2856,6 +3041,56 @@
         </is>
       </c>
       <c r="B20" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:44:24</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:49:58</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:55:19</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:56:54</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2026-01-18T17:00:01</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
         <v>1399</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pridani send_bool do USER_WITH_EMAIL + tlacitko co tuto hodnotu meni
</commit_message>
<xml_diff>
--- a/produkty.xlsx
+++ b/produkty.xlsx
@@ -174,12 +174,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'27 - PlayStation 4 Slim 500GB'!$A$9:$A$16</f>
+              <f>'27 - PlayStation 4 Slim 500GB'!$A$9:$A$17</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'27 - PlayStation 4 Slim 500GB'!$B$9:$B$16</f>
+              <f>'27 - PlayStation 4 Slim 500GB'!$B$9:$B$17</f>
             </numRef>
           </val>
         </ser>
@@ -564,7 +564,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -748,6 +748,16 @@
         <v>6636</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2026-01-24T20:37:37</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>6636</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>